<commit_message>
Added capability for legal entity
</commit_message>
<xml_diff>
--- a/excel_output/excel_files_20240930_113906/employee_performance_metrics.xlsx
+++ b/excel_output/excel_files_20240930_113906/employee_performance_metrics.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltacapita-my.sharepoint.com/personal/john_elliott_deltacapita_com/Documents/Desktop/EXCEL_PROJECT/excel_output/excel_files_20240930_113906/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_C2F2812DF0B0D757203C343058F65602441D9D85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{752F8E5D-96F3-4DCE-8794-838E262DA130}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -67,11 +73,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,13 +141,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -179,7 +193,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -213,6 +227,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -247,9 +262,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -422,14 +438,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +469,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45323</v>
       </c>
@@ -463,7 +486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45323</v>
       </c>
@@ -480,7 +503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45323</v>
       </c>
@@ -497,7 +520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45323</v>
       </c>
@@ -514,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45323</v>
       </c>
@@ -531,7 +554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45323</v>
       </c>
@@ -548,7 +571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45323</v>
       </c>
@@ -565,7 +588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45323</v>
       </c>
@@ -582,7 +605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45323</v>
       </c>
@@ -599,7 +622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45323</v>
       </c>
@@ -616,7 +639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45323</v>
       </c>
@@ -633,7 +656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45352</v>
       </c>
@@ -650,7 +673,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45352</v>
       </c>
@@ -667,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45352</v>
       </c>
@@ -684,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45352</v>
       </c>
@@ -701,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45352</v>
       </c>
@@ -718,7 +741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45352</v>
       </c>
@@ -735,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45352</v>
       </c>
@@ -752,7 +775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45352</v>
       </c>
@@ -769,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45352</v>
       </c>
@@ -786,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45352</v>
       </c>
@@ -803,7 +826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45352</v>
       </c>
@@ -820,7 +843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45383</v>
       </c>
@@ -837,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45383</v>
       </c>
@@ -854,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45383</v>
       </c>
@@ -871,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45383</v>
       </c>
@@ -888,7 +911,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45383</v>
       </c>
@@ -905,7 +928,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45383</v>
       </c>
@@ -922,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45383</v>
       </c>
@@ -939,7 +962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45383</v>
       </c>
@@ -956,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45383</v>
       </c>
@@ -973,7 +996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45383</v>
       </c>
@@ -990,7 +1013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>45383</v>
       </c>
@@ -1007,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>45413</v>
       </c>
@@ -1024,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>45413</v>
       </c>
@@ -1041,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>45413</v>
       </c>
@@ -1058,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>45413</v>
       </c>
@@ -1075,7 +1098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>45413</v>
       </c>
@@ -1092,7 +1115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>45413</v>
       </c>
@@ -1109,7 +1132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>45413</v>
       </c>
@@ -1126,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45413</v>
       </c>
@@ -1143,7 +1166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45413</v>
       </c>
@@ -1160,7 +1183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>45413</v>
       </c>
@@ -1177,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45413</v>
       </c>
@@ -1194,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45444</v>
       </c>
@@ -1211,7 +1234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45444</v>
       </c>
@@ -1228,7 +1251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45444</v>
       </c>
@@ -1245,7 +1268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45444</v>
       </c>
@@ -1262,7 +1285,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>45444</v>
       </c>
@@ -1279,7 +1302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>45444</v>
       </c>
@@ -1296,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45444</v>
       </c>
@@ -1313,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45444</v>
       </c>
@@ -1330,7 +1353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>45444</v>
       </c>
@@ -1347,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>45444</v>
       </c>
@@ -1364,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>45444</v>
       </c>
@@ -1381,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>45474</v>
       </c>
@@ -1398,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>45474</v>
       </c>
@@ -1415,7 +1438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>45474</v>
       </c>
@@ -1432,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>45474</v>
       </c>
@@ -1449,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>45474</v>
       </c>
@@ -1466,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>45474</v>
       </c>
@@ -1483,7 +1506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>45474</v>
       </c>
@@ -1500,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>45474</v>
       </c>
@@ -1517,7 +1540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>45474</v>
       </c>
@@ -1534,7 +1557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>45474</v>
       </c>
@@ -1551,7 +1574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>45474</v>
       </c>
@@ -1568,7 +1591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>45505</v>
       </c>
@@ -1585,7 +1608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>45505</v>
       </c>
@@ -1602,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>45505</v>
       </c>
@@ -1619,7 +1642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>45505</v>
       </c>
@@ -1636,7 +1659,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>45505</v>
       </c>
@@ -1653,7 +1676,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>45505</v>
       </c>
@@ -1670,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:5">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>45505</v>
       </c>
@@ -1687,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:5">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>45505</v>
       </c>
@@ -1704,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>45505</v>
       </c>
@@ -1721,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>45505</v>
       </c>
@@ -1738,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>45505</v>
       </c>
@@ -1755,7 +1778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>45536</v>
       </c>
@@ -1772,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>45536</v>
       </c>
@@ -1789,7 +1812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>45536</v>
       </c>
@@ -1806,7 +1829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:5">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>45536</v>
       </c>
@@ -1823,7 +1846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:5">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>45536</v>
       </c>
@@ -1840,7 +1863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:5">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>45536</v>
       </c>
@@ -1857,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:5">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>45536</v>
       </c>
@@ -1874,7 +1897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>45536</v>
       </c>
@@ -1891,7 +1914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:5">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>45536</v>
       </c>
@@ -1908,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>45536</v>
       </c>
@@ -1925,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>45536</v>
       </c>

</xml_diff>